<commit_message>
Modal de errores y cantidad máxima de filas por excel en subidas masivas
</commit_message>
<xml_diff>
--- a/public/templates/Plantilla_cesar_usuarios.xlsx
+++ b/public/templates/Plantilla_cesar_usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\gestor\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED0D453-CEE4-4E83-A245-064769DE2905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2571F29E-0D17-4592-98FC-75BE9FD780D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
     <t xml:space="preserve">DOCUMENTO </t>
   </si>
   <si>
-    <t>FECHA DE CESE (OPCIONAL): 2020-12-10</t>
+    <t>FECHA DE CESE (OPCIONAL)</t>
   </si>
 </sst>
 </file>
@@ -329,7 +329,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>